<commit_message>
MEPs Hoop + Tableau longueur tubes
+ screen simulation
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/Frame_Production/Commande_longueur_tubes.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/Frame_Production/Commande_longueur_tubes.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\negre\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\negre\Documents\EPSA\ELIZ-2021\FR_Frame_Body\FR_A0100 (Frame)\Frame_Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E96C654-AD8C-44C5-BA02-34E05BF50979}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC681081-5C66-4765-B7DA-F75D7345AFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11955" yWindow="1410" windowWidth="12510" windowHeight="11265" xr2:uid="{82C8B06B-864A-4419-9C90-31493652AB52}"/>
+    <workbookView xWindow="11955" yWindow="1410" windowWidth="12510" windowHeight="11265" activeTab="1" xr2:uid="{82C8B06B-864A-4419-9C90-31493652AB52}"/>
   </bookViews>
   <sheets>
     <sheet name="Bilan" sheetId="8" r:id="rId1"/>
-    <sheet name="30x2" sheetId="1" r:id="rId2"/>
-    <sheet name="28x1.5" sheetId="6" r:id="rId3"/>
-    <sheet name="25x1.5" sheetId="3" r:id="rId4"/>
-    <sheet name="20x1.5" sheetId="4" r:id="rId5"/>
-    <sheet name="15x1.5" sheetId="5" r:id="rId6"/>
-    <sheet name="28x2" sheetId="2" r:id="rId7"/>
-    <sheet name="25x2" sheetId="7" r:id="rId8"/>
+    <sheet name="Bilan_final" sheetId="9" r:id="rId2"/>
+    <sheet name="30x2" sheetId="1" r:id="rId3"/>
+    <sheet name="28x1.5" sheetId="6" r:id="rId4"/>
+    <sheet name="25x1.5" sheetId="3" r:id="rId5"/>
+    <sheet name="20x1.5" sheetId="4" r:id="rId6"/>
+    <sheet name="15x1.5" sheetId="5" r:id="rId7"/>
+    <sheet name="28x2" sheetId="2" r:id="rId8"/>
+    <sheet name="25x2" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
   <si>
     <t>front hoop</t>
   </si>
@@ -101,13 +102,190 @@
   </si>
   <si>
     <t>longueur à commander (m)</t>
+  </si>
+  <si>
+    <t>Couleur</t>
+  </si>
+  <si>
+    <t>Taille du tube</t>
+  </si>
+  <si>
+    <t>Nombre de tubes</t>
+  </si>
+  <si>
+    <t>Longueur du tube</t>
+  </si>
+  <si>
+    <t>Longueur totale (mm)</t>
+  </si>
+  <si>
+    <t>Masse (kg)</t>
+  </si>
+  <si>
+    <t>2x</t>
+  </si>
+  <si>
+    <t>1x</t>
+  </si>
+  <si>
+    <t>4x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">360mm </t>
+  </si>
+  <si>
+    <t>1720mm</t>
+  </si>
+  <si>
+    <t>2646mm</t>
+  </si>
+  <si>
+    <t>510mm</t>
+  </si>
+  <si>
+    <t>665mm</t>
+  </si>
+  <si>
+    <t>433mm</t>
+  </si>
+  <si>
+    <t>807mm</t>
+  </si>
+  <si>
+    <t>310mm</t>
+  </si>
+  <si>
+    <t>755mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">605mm </t>
+  </si>
+  <si>
+    <t>138mm</t>
+  </si>
+  <si>
+    <t>464mm</t>
+  </si>
+  <si>
+    <t>380mm</t>
+  </si>
+  <si>
+    <t>236mm</t>
+  </si>
+  <si>
+    <t>330mm</t>
+  </si>
+  <si>
+    <t>338mm</t>
+  </si>
+  <si>
+    <t>140mm</t>
+  </si>
+  <si>
+    <t>273mm</t>
+  </si>
+  <si>
+    <t>258mm</t>
+  </si>
+  <si>
+    <t>414mm</t>
+  </si>
+  <si>
+    <t>577mm</t>
+  </si>
+  <si>
+    <t>502mm</t>
+  </si>
+  <si>
+    <t>574mm</t>
+  </si>
+  <si>
+    <t>320mm</t>
+  </si>
+  <si>
+    <t>859mm</t>
+  </si>
+  <si>
+    <t>203mm</t>
+  </si>
+  <si>
+    <t>268mm</t>
+  </si>
+  <si>
+    <t>270mm</t>
+  </si>
+  <si>
+    <t>353mm</t>
+  </si>
+  <si>
+    <t>159mm</t>
+  </si>
+  <si>
+    <t>361mm</t>
+  </si>
+  <si>
+    <t>205mm</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>300mm</t>
+  </si>
+  <si>
+    <t>400mm</t>
+  </si>
+  <si>
+    <t>609mm</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>461mm</t>
+  </si>
+  <si>
+    <t>279mm</t>
+  </si>
+  <si>
+    <t>652mm</t>
+  </si>
+  <si>
+    <t>64mm</t>
+  </si>
+  <si>
+    <t>223mm</t>
+  </si>
+  <si>
+    <t>448mm</t>
+  </si>
+  <si>
+    <t>339mm</t>
+  </si>
+  <si>
+    <t>649mm</t>
+  </si>
+  <si>
+    <t>520mm</t>
+  </si>
+  <si>
+    <t>81mm</t>
+  </si>
+  <si>
+    <t>50mm</t>
+  </si>
+  <si>
+    <t>105mm</t>
+  </si>
+  <si>
+    <t>Masse totale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,16 +293,72 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -132,19 +366,254 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF66CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -455,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3519A1-2F84-4698-9F0B-76122CA2F9EB}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,13 +952,13 @@
       </c>
       <c r="C2">
         <f>B2/1000*(1+F2)</f>
-        <v>4.8026</v>
+        <v>4.3659999999999997</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
       </c>
       <c r="F2" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -502,7 +971,7 @@
       </c>
       <c r="C3">
         <f>B3/1000*(1+F2)</f>
-        <v>11.473000000000001</v>
+        <v>10.43</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -515,7 +984,7 @@
       </c>
       <c r="C4">
         <f>B4/1000*(1+F2)</f>
-        <v>11.477399999999999</v>
+        <v>10.433999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -528,7 +997,7 @@
       </c>
       <c r="C5">
         <f>B5/1000*(1+F2)</f>
-        <v>9.1476000000000024</v>
+        <v>8.3160000000000007</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -541,7 +1010,7 @@
       </c>
       <c r="C6">
         <f>B6/1000*(1+F2)</f>
-        <v>6.711100000000001</v>
+        <v>6.101</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -554,7 +1023,7 @@
       </c>
       <c r="C7">
         <f>B7/1000*(1+F2)</f>
-        <v>0.17820000000000003</v>
+        <v>0.16200000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -567,7 +1036,7 @@
       </c>
       <c r="C8">
         <f>B8/1000*(1+F2)</f>
-        <v>0.34100000000000003</v>
+        <v>0.31</v>
       </c>
     </row>
   </sheetData>
@@ -576,11 +1045,616 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C998DDB5-B097-4D41-B0C8-BC612859258C}">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="3">
+        <v>4366</v>
+      </c>
+      <c r="G2" s="3">
+        <v>6.3650000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="12">
+        <v>10430</v>
+      </c>
+      <c r="G3" s="14">
+        <v>10.234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="12">
+        <v>10434</v>
+      </c>
+      <c r="G8" s="12">
+        <v>9.6820000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12">
+        <v>8316</v>
+      </c>
+      <c r="G16" s="12">
+        <v>5.6840000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="12">
+        <v>6101</v>
+      </c>
+      <c r="G23" s="12">
+        <v>3.0449999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
+      <c r="B28" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="12">
+        <v>162</v>
+      </c>
+      <c r="G28" s="12">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
+      <c r="B30" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" s="12">
+        <v>310</v>
+      </c>
+      <c r="G30" s="12">
+        <v>0.34399999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="31"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32" s="3">
+        <f>SUM(G2:G31)</f>
+        <v>35.561</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="G16:G22"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="G23:G27"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:F22"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="G3:G7"/>
+    <mergeCell ref="F8:F15"/>
+    <mergeCell ref="G8:G15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="C8:C14"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F3:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F0D07D-6188-49F9-BB47-DEF398DF11AD}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,12 +1699,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D7A799-0911-4DE9-A394-D04651BB0FF0}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,12 +1759,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{818AAA5E-5A70-4E6D-BA21-6C990B825B07}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,12 +1810,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBA8BFF-23CE-4D7C-9529-471DCFFACD4F}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,12 +1870,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D162A08-1477-4F6B-8658-D1849AE699EC}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,12 +1939,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F3E345E-EE76-4CD4-B9EA-61A45D17A871}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,12 +1981,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC901396-2893-45BB-A0E0-ED22903DAD5D}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>